<commit_message>
added addr data to test addr formatting button
</commit_message>
<xml_diff>
--- a/nrFixer Guide.xlsx
+++ b/nrFixer Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\Documents\Personal\Military\S1\nrFixer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5527E3-AD9E-41D8-95B4-F719A723B0A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2106DD87-28AD-43F5-BA82-D94B27040768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="92">
   <si>
     <t>RANK</t>
   </si>
@@ -314,10 +314,7 @@
     <t>DOI</t>
   </si>
   <si>
-    <t>ELIGIBLITY</t>
-  </si>
-  <si>
-    <t>PERFORMANCE</t>
+    <t>ADDR</t>
   </si>
 </sst>
 </file>
@@ -637,10 +634,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D3AD263-2CFC-4E5F-B56F-091E6A24DD04}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +711,7 @@
         <v>89</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:C11" si="0">C7+1</f>
+        <f t="shared" ref="C8:C12" si="0">C7+1</f>
         <v>4</v>
       </c>
       <c r="E8">
@@ -743,18 +740,6 @@
       </c>
       <c r="E10">
         <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="E11">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>